<commit_message>
export to excel ws report 567
</commit_message>
<xml_diff>
--- a/data/ws4_output.xlsx
+++ b/data/ws4_output.xlsx
@@ -89,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -500,6 +500,21 @@
       <top/>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,7 +643,7 @@
     <xf borderId="34" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="31" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="27" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="35" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Обычный" xfId="0"/>
@@ -1040,7 +1055,7 @@
       </c>
       <c r="X1" s="19" t="inlineStr">
         <is>
-          <t>2020-06-13</t>
+          <t>2020-06-14</t>
         </is>
       </c>
       <c r="Y1" s="20" t="n"/>
@@ -1052,7 +1067,7 @@
       </c>
       <c r="AB1" s="22" t="inlineStr">
         <is>
-          <t>2020-07-13</t>
+          <t>2020-07-14</t>
         </is>
       </c>
       <c r="AC1" s="22" t="n"/>
@@ -1371,25 +1386,19 @@
     <row customHeight="1" ht="16.5" r="5">
       <c r="A5" s="37" t="inlineStr">
         <is>
-          <t>2020-06-13</t>
+          <t>2020-06-14</t>
         </is>
       </c>
       <c r="B5" s="37" t="n">
-        <v>444</v>
+        <v>1131</v>
       </c>
       <c r="C5" s="37" t="inlineStr"/>
       <c r="D5" s="37" t="n">
-        <v>444</v>
+        <v>1131</v>
       </c>
       <c r="E5" s="37" t="inlineStr"/>
-      <c r="F5" s="37" t="inlineStr">
-        <is>
-          <t>690(690)</t>
-        </is>
-      </c>
-      <c r="G5" s="37" t="n">
-        <v>5313</v>
-      </c>
+      <c r="F5" s="37" t="inlineStr"/>
+      <c r="G5" s="37" t="n"/>
       <c r="H5" s="37" t="n"/>
       <c r="I5" s="37" t="n"/>
       <c r="J5" s="37" t="n"/>
@@ -1398,12 +1407,8 @@
       <c r="M5" s="37" t="n"/>
       <c r="N5" s="37" t="n"/>
       <c r="O5" s="37" t="n"/>
-      <c r="P5" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="37" t="n">
-        <v>16</v>
-      </c>
+      <c r="P5" s="37" t="n"/>
+      <c r="Q5" s="37" t="n"/>
       <c r="R5" s="37" t="n"/>
       <c r="S5" s="37" t="n"/>
       <c r="T5" s="37" t="n"/>
@@ -1412,16 +1417,12 @@
       <c r="W5" s="37" t="n"/>
       <c r="X5" s="37" t="n"/>
       <c r="Y5" s="37" t="n"/>
-      <c r="Z5" s="37" t="inlineStr"/>
-      <c r="AA5" s="37" t="inlineStr"/>
+      <c r="Z5" s="37" t="n"/>
+      <c r="AA5" s="37" t="n"/>
       <c r="AB5" s="37" t="n"/>
       <c r="AC5" s="37" t="n"/>
-      <c r="AD5" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="37" t="n">
-        <v>9</v>
-      </c>
+      <c r="AD5" s="37" t="n"/>
+      <c r="AE5" s="37" t="n"/>
       <c r="AF5" s="37" t="n">
         <v>1131</v>
       </c>
@@ -1435,7 +1436,7 @@
     <row customHeight="1" ht="16.5" r="6">
       <c r="A6" s="37" t="inlineStr">
         <is>
-          <t>2020-06-14</t>
+          <t>2020-06-15</t>
         </is>
       </c>
       <c r="B6" s="37" t="n">
@@ -1456,8 +1457,8 @@
       <c r="M6" s="37" t="n"/>
       <c r="N6" s="37" t="n"/>
       <c r="O6" s="37" t="n"/>
-      <c r="P6" s="37" t="inlineStr"/>
-      <c r="Q6" s="37" t="inlineStr"/>
+      <c r="P6" s="37" t="n"/>
+      <c r="Q6" s="37" t="n"/>
       <c r="R6" s="37" t="n"/>
       <c r="S6" s="37" t="n"/>
       <c r="T6" s="37" t="n"/>
@@ -1466,12 +1467,12 @@
       <c r="W6" s="37" t="n"/>
       <c r="X6" s="37" t="n"/>
       <c r="Y6" s="37" t="n"/>
-      <c r="Z6" s="37" t="inlineStr"/>
-      <c r="AA6" s="37" t="inlineStr"/>
+      <c r="Z6" s="37" t="n"/>
+      <c r="AA6" s="37" t="n"/>
       <c r="AB6" s="37" t="n"/>
       <c r="AC6" s="37" t="n"/>
-      <c r="AD6" s="37" t="inlineStr"/>
-      <c r="AE6" s="37" t="inlineStr"/>
+      <c r="AD6" s="37" t="n"/>
+      <c r="AE6" s="37" t="n"/>
       <c r="AF6" s="37" t="n">
         <v>1131</v>
       </c>
@@ -1485,7 +1486,7 @@
     <row customHeight="1" ht="16.5" r="7">
       <c r="A7" s="37" t="inlineStr">
         <is>
-          <t>2020-06-15</t>
+          <t>2020-06-16</t>
         </is>
       </c>
       <c r="B7" s="37" t="n">
@@ -1506,8 +1507,8 @@
       <c r="M7" s="37" t="n"/>
       <c r="N7" s="37" t="n"/>
       <c r="O7" s="37" t="n"/>
-      <c r="P7" s="37" t="inlineStr"/>
-      <c r="Q7" s="37" t="inlineStr"/>
+      <c r="P7" s="37" t="n"/>
+      <c r="Q7" s="37" t="n"/>
       <c r="R7" s="37" t="n"/>
       <c r="S7" s="37" t="n"/>
       <c r="T7" s="37" t="n"/>
@@ -1516,12 +1517,12 @@
       <c r="W7" s="37" t="n"/>
       <c r="X7" s="37" t="n"/>
       <c r="Y7" s="37" t="n"/>
-      <c r="Z7" s="37" t="inlineStr"/>
-      <c r="AA7" s="37" t="inlineStr"/>
+      <c r="Z7" s="37" t="n"/>
+      <c r="AA7" s="37" t="n"/>
       <c r="AB7" s="37" t="n"/>
       <c r="AC7" s="37" t="n"/>
-      <c r="AD7" s="37" t="inlineStr"/>
-      <c r="AE7" s="37" t="inlineStr"/>
+      <c r="AD7" s="37" t="n"/>
+      <c r="AE7" s="37" t="n"/>
       <c r="AF7" s="37" t="n">
         <v>1131</v>
       </c>
@@ -1535,7 +1536,7 @@
     <row customHeight="1" ht="16.5" r="8">
       <c r="A8" s="37" t="inlineStr">
         <is>
-          <t>2020-06-16</t>
+          <t>2020-06-17</t>
         </is>
       </c>
       <c r="B8" s="37" t="n">
@@ -1552,12 +1553,20 @@
       <c r="I8" s="37" t="n"/>
       <c r="J8" s="37" t="n"/>
       <c r="K8" s="37" t="n"/>
-      <c r="L8" s="37" t="inlineStr"/>
+      <c r="L8" s="37" t="inlineStr">
+        <is>
+          <t>(632)</t>
+        </is>
+      </c>
       <c r="M8" s="37" t="n"/>
       <c r="N8" s="37" t="n"/>
       <c r="O8" s="37" t="n"/>
-      <c r="P8" s="37" t="inlineStr"/>
-      <c r="Q8" s="37" t="inlineStr"/>
+      <c r="P8" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="37" t="n">
+        <v>14</v>
+      </c>
       <c r="R8" s="37" t="n"/>
       <c r="S8" s="37" t="n"/>
       <c r="T8" s="37" t="n"/>
@@ -1566,34 +1575,38 @@
       <c r="W8" s="37" t="n"/>
       <c r="X8" s="37" t="n"/>
       <c r="Y8" s="37" t="n"/>
-      <c r="Z8" s="37" t="inlineStr"/>
-      <c r="AA8" s="37" t="inlineStr"/>
+      <c r="Z8" s="37" t="n"/>
+      <c r="AA8" s="37" t="n"/>
       <c r="AB8" s="37" t="n"/>
       <c r="AC8" s="37" t="n"/>
-      <c r="AD8" s="37" t="inlineStr"/>
-      <c r="AE8" s="37" t="inlineStr"/>
+      <c r="AD8" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="37" t="n">
+        <v>11</v>
+      </c>
       <c r="AF8" s="37" t="n">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="AG8" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH8" s="37" t="n">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="9">
       <c r="A9" s="37" t="inlineStr">
         <is>
-          <t>2020-06-17</t>
+          <t>2020-06-18</t>
         </is>
       </c>
       <c r="B9" s="37" t="n">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C9" s="37" t="inlineStr"/>
       <c r="D9" s="37" t="n">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E9" s="37" t="inlineStr"/>
       <c r="F9" s="37" t="inlineStr"/>
@@ -1604,18 +1617,14 @@
       <c r="K9" s="37" t="n"/>
       <c r="L9" s="37" t="inlineStr">
         <is>
-          <t>(632)</t>
+          <t>632</t>
         </is>
       </c>
       <c r="M9" s="37" t="n"/>
       <c r="N9" s="37" t="n"/>
       <c r="O9" s="37" t="n"/>
-      <c r="P9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="37" t="n">
-        <v>14</v>
-      </c>
+      <c r="P9" s="37" t="n"/>
+      <c r="Q9" s="37" t="n"/>
       <c r="R9" s="37" t="n"/>
       <c r="S9" s="37" t="n"/>
       <c r="T9" s="37" t="n"/>
@@ -1624,56 +1633,54 @@
       <c r="W9" s="37" t="n"/>
       <c r="X9" s="37" t="n"/>
       <c r="Y9" s="37" t="n"/>
-      <c r="Z9" s="37" t="inlineStr"/>
-      <c r="AA9" s="37" t="inlineStr"/>
+      <c r="Z9" s="37" t="n"/>
+      <c r="AA9" s="37" t="n"/>
       <c r="AB9" s="37" t="n"/>
       <c r="AC9" s="37" t="n"/>
-      <c r="AD9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="37" t="n">
-        <v>11</v>
-      </c>
+      <c r="AD9" s="37" t="n"/>
+      <c r="AE9" s="37" t="n"/>
       <c r="AF9" s="37" t="n">
-        <v>1129</v>
+        <v>497</v>
       </c>
       <c r="AG9" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH9" s="37" t="n">
-        <v>1129</v>
+        <v>497</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="10">
       <c r="A10" s="37" t="inlineStr">
         <is>
-          <t>2020-06-18</t>
+          <t>2020-06-19</t>
         </is>
       </c>
       <c r="B10" s="37" t="n">
-        <v>1129</v>
+        <v>497</v>
       </c>
       <c r="C10" s="37" t="inlineStr"/>
       <c r="D10" s="37" t="n">
-        <v>1129</v>
+        <v>497</v>
       </c>
       <c r="E10" s="37" t="inlineStr"/>
-      <c r="F10" s="37" t="inlineStr"/>
-      <c r="G10" s="37" t="n"/>
+      <c r="F10" s="37" t="inlineStr">
+        <is>
+          <t>(579)</t>
+        </is>
+      </c>
+      <c r="G10" s="37" t="n">
+        <v>4458.6</v>
+      </c>
       <c r="H10" s="37" t="n"/>
       <c r="I10" s="37" t="n"/>
       <c r="J10" s="37" t="n"/>
       <c r="K10" s="37" t="n"/>
-      <c r="L10" s="37" t="inlineStr">
-        <is>
-          <t>632</t>
-        </is>
-      </c>
+      <c r="L10" s="37" t="inlineStr"/>
       <c r="M10" s="37" t="n"/>
       <c r="N10" s="37" t="n"/>
       <c r="O10" s="37" t="n"/>
-      <c r="P10" s="37" t="inlineStr"/>
-      <c r="Q10" s="37" t="inlineStr"/>
+      <c r="P10" s="37" t="n"/>
+      <c r="Q10" s="37" t="n"/>
       <c r="R10" s="37" t="n"/>
       <c r="S10" s="37" t="n"/>
       <c r="T10" s="37" t="n"/>
@@ -1682,44 +1689,46 @@
       <c r="W10" s="37" t="n"/>
       <c r="X10" s="37" t="n"/>
       <c r="Y10" s="37" t="n"/>
-      <c r="Z10" s="37" t="inlineStr"/>
-      <c r="AA10" s="37" t="inlineStr"/>
+      <c r="Z10" s="37" t="n"/>
+      <c r="AA10" s="37" t="n"/>
       <c r="AB10" s="37" t="n"/>
       <c r="AC10" s="37" t="n"/>
-      <c r="AD10" s="37" t="inlineStr"/>
-      <c r="AE10" s="37" t="inlineStr"/>
+      <c r="AD10" s="37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="37" t="n">
+        <v>25</v>
+      </c>
       <c r="AF10" s="37" t="n">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="AG10" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH10" s="37" t="n">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="11">
       <c r="A11" s="37" t="inlineStr">
         <is>
-          <t>2020-06-19</t>
+          <t>2020-06-20</t>
         </is>
       </c>
       <c r="B11" s="37" t="n">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C11" s="37" t="inlineStr"/>
       <c r="D11" s="37" t="n">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E11" s="37" t="inlineStr"/>
       <c r="F11" s="37" t="inlineStr">
         <is>
-          <t>(579)</t>
-        </is>
-      </c>
-      <c r="G11" s="37" t="n">
-        <v>4458.6</v>
-      </c>
+          <t>579</t>
+        </is>
+      </c>
+      <c r="G11" s="37" t="n"/>
       <c r="H11" s="37" t="n"/>
       <c r="I11" s="37" t="n"/>
       <c r="J11" s="37" t="n"/>
@@ -1728,8 +1737,12 @@
       <c r="M11" s="37" t="n"/>
       <c r="N11" s="37" t="n"/>
       <c r="O11" s="37" t="n"/>
-      <c r="P11" s="37" t="inlineStr"/>
-      <c r="Q11" s="37" t="inlineStr"/>
+      <c r="P11" s="37" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="37" t="n">
+        <v>23</v>
+      </c>
       <c r="R11" s="37" t="n"/>
       <c r="S11" s="37" t="n"/>
       <c r="T11" s="37" t="n"/>
@@ -1738,45 +1751,37 @@
       <c r="W11" s="37" t="n"/>
       <c r="X11" s="37" t="n"/>
       <c r="Y11" s="37" t="n"/>
-      <c r="Z11" s="37" t="inlineStr"/>
-      <c r="AA11" s="37" t="inlineStr"/>
+      <c r="Z11" s="37" t="n"/>
+      <c r="AA11" s="37" t="n"/>
       <c r="AB11" s="37" t="n"/>
       <c r="AC11" s="37" t="n"/>
-      <c r="AD11" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="37" t="n">
-        <v>25</v>
-      </c>
+      <c r="AD11" s="37" t="n"/>
+      <c r="AE11" s="37" t="n"/>
       <c r="AF11" s="37" t="n">
-        <v>494</v>
+        <v>1070</v>
       </c>
       <c r="AG11" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH11" s="37" t="n">
-        <v>494</v>
+        <v>1070</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="12">
       <c r="A12" s="37" t="inlineStr">
         <is>
-          <t>2020-06-20</t>
+          <t>2020-06-21</t>
         </is>
       </c>
       <c r="B12" s="37" t="n">
-        <v>494</v>
+        <v>1070</v>
       </c>
       <c r="C12" s="37" t="inlineStr"/>
       <c r="D12" s="37" t="n">
-        <v>494</v>
+        <v>1070</v>
       </c>
       <c r="E12" s="37" t="inlineStr"/>
-      <c r="F12" s="37" t="inlineStr">
-        <is>
-          <t>579</t>
-        </is>
-      </c>
+      <c r="F12" s="37" t="inlineStr"/>
       <c r="G12" s="37" t="n"/>
       <c r="H12" s="37" t="n"/>
       <c r="I12" s="37" t="n"/>
@@ -1786,12 +1791,8 @@
       <c r="M12" s="37" t="n"/>
       <c r="N12" s="37" t="n"/>
       <c r="O12" s="37" t="n"/>
-      <c r="P12" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="37" t="n">
-        <v>23</v>
-      </c>
+      <c r="P12" s="37" t="n"/>
+      <c r="Q12" s="37" t="n"/>
       <c r="R12" s="37" t="n"/>
       <c r="S12" s="37" t="n"/>
       <c r="T12" s="37" t="n"/>
@@ -1800,12 +1801,12 @@
       <c r="W12" s="37" t="n"/>
       <c r="X12" s="37" t="n"/>
       <c r="Y12" s="37" t="n"/>
-      <c r="Z12" s="37" t="inlineStr"/>
-      <c r="AA12" s="37" t="inlineStr"/>
+      <c r="Z12" s="37" t="n"/>
+      <c r="AA12" s="37" t="n"/>
       <c r="AB12" s="37" t="n"/>
       <c r="AC12" s="37" t="n"/>
-      <c r="AD12" s="37" t="inlineStr"/>
-      <c r="AE12" s="37" t="inlineStr"/>
+      <c r="AD12" s="37" t="n"/>
+      <c r="AE12" s="37" t="n"/>
       <c r="AF12" s="37" t="n">
         <v>1070</v>
       </c>
@@ -1819,7 +1820,7 @@
     <row customHeight="1" ht="16.5" r="13">
       <c r="A13" s="37" t="inlineStr">
         <is>
-          <t>2020-06-21</t>
+          <t>2020-06-22</t>
         </is>
       </c>
       <c r="B13" s="37" t="n">
@@ -1840,8 +1841,8 @@
       <c r="M13" s="37" t="n"/>
       <c r="N13" s="37" t="n"/>
       <c r="O13" s="37" t="n"/>
-      <c r="P13" s="37" t="inlineStr"/>
-      <c r="Q13" s="37" t="inlineStr"/>
+      <c r="P13" s="37" t="n"/>
+      <c r="Q13" s="37" t="n"/>
       <c r="R13" s="37" t="n"/>
       <c r="S13" s="37" t="n"/>
       <c r="T13" s="37" t="n"/>
@@ -1850,12 +1851,12 @@
       <c r="W13" s="37" t="n"/>
       <c r="X13" s="37" t="n"/>
       <c r="Y13" s="37" t="n"/>
-      <c r="Z13" s="37" t="inlineStr"/>
-      <c r="AA13" s="37" t="inlineStr"/>
+      <c r="Z13" s="37" t="n"/>
+      <c r="AA13" s="37" t="n"/>
       <c r="AB13" s="37" t="n"/>
       <c r="AC13" s="37" t="n"/>
-      <c r="AD13" s="37" t="inlineStr"/>
-      <c r="AE13" s="37" t="inlineStr"/>
+      <c r="AD13" s="37" t="n"/>
+      <c r="AE13" s="37" t="n"/>
       <c r="AF13" s="37" t="n">
         <v>1070</v>
       </c>
@@ -1869,7 +1870,7 @@
     <row customHeight="1" ht="16.5" r="14">
       <c r="A14" s="37" t="inlineStr">
         <is>
-          <t>2020-06-22</t>
+          <t>2020-06-23</t>
         </is>
       </c>
       <c r="B14" s="37" t="n">
@@ -1890,8 +1891,8 @@
       <c r="M14" s="37" t="n"/>
       <c r="N14" s="37" t="n"/>
       <c r="O14" s="37" t="n"/>
-      <c r="P14" s="37" t="inlineStr"/>
-      <c r="Q14" s="37" t="inlineStr"/>
+      <c r="P14" s="37" t="n"/>
+      <c r="Q14" s="37" t="n"/>
       <c r="R14" s="37" t="n"/>
       <c r="S14" s="37" t="n"/>
       <c r="T14" s="37" t="n"/>
@@ -1900,12 +1901,12 @@
       <c r="W14" s="37" t="n"/>
       <c r="X14" s="37" t="n"/>
       <c r="Y14" s="37" t="n"/>
-      <c r="Z14" s="37" t="inlineStr"/>
-      <c r="AA14" s="37" t="inlineStr"/>
+      <c r="Z14" s="37" t="n"/>
+      <c r="AA14" s="37" t="n"/>
       <c r="AB14" s="37" t="n"/>
       <c r="AC14" s="37" t="n"/>
-      <c r="AD14" s="37" t="inlineStr"/>
-      <c r="AE14" s="37" t="inlineStr"/>
+      <c r="AD14" s="37" t="n"/>
+      <c r="AE14" s="37" t="n"/>
       <c r="AF14" s="37" t="n">
         <v>1070</v>
       </c>
@@ -1919,7 +1920,7 @@
     <row customHeight="1" ht="16.5" r="15">
       <c r="A15" s="37" t="inlineStr">
         <is>
-          <t>2020-06-23</t>
+          <t>2020-06-24</t>
         </is>
       </c>
       <c r="B15" s="37" t="n">
@@ -1940,8 +1941,12 @@
       <c r="M15" s="37" t="n"/>
       <c r="N15" s="37" t="n"/>
       <c r="O15" s="37" t="n"/>
-      <c r="P15" s="37" t="inlineStr"/>
-      <c r="Q15" s="37" t="inlineStr"/>
+      <c r="P15" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="37" t="n">
+        <v>19</v>
+      </c>
       <c r="R15" s="37" t="n"/>
       <c r="S15" s="37" t="n"/>
       <c r="T15" s="37" t="n"/>
@@ -1950,43 +1955,59 @@
       <c r="W15" s="37" t="n"/>
       <c r="X15" s="37" t="n"/>
       <c r="Y15" s="37" t="n"/>
-      <c r="Z15" s="37" t="inlineStr"/>
-      <c r="AA15" s="37" t="inlineStr"/>
+      <c r="Z15" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA15" s="37" t="n">
+        <v>123</v>
+      </c>
       <c r="AB15" s="37" t="n"/>
       <c r="AC15" s="37" t="n"/>
-      <c r="AD15" s="37" t="inlineStr"/>
-      <c r="AE15" s="37" t="inlineStr"/>
+      <c r="AD15" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="37" t="n">
+        <v>10</v>
+      </c>
       <c r="AF15" s="37" t="n">
-        <v>1070</v>
+        <v>1057</v>
       </c>
       <c r="AG15" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH15" s="37" t="n">
-        <v>1070</v>
+        <v>1057</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="16">
       <c r="A16" s="37" t="inlineStr">
         <is>
-          <t>2020-06-24</t>
+          <t>2020-06-25</t>
         </is>
       </c>
       <c r="B16" s="37" t="n">
-        <v>1070</v>
+        <v>1057</v>
       </c>
       <c r="C16" s="37" t="inlineStr"/>
       <c r="D16" s="37" t="n">
-        <v>1070</v>
+        <v>1057</v>
       </c>
       <c r="E16" s="37" t="inlineStr"/>
-      <c r="F16" s="37" t="inlineStr"/>
+      <c r="F16" s="37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="G16" s="37" t="n"/>
       <c r="H16" s="37" t="n"/>
       <c r="I16" s="37" t="n"/>
       <c r="J16" s="37" t="n"/>
       <c r="K16" s="37" t="n"/>
-      <c r="L16" s="37" t="inlineStr"/>
+      <c r="L16" s="37" t="inlineStr">
+        <is>
+          <t>682(682)</t>
+        </is>
+      </c>
       <c r="M16" s="37" t="n"/>
       <c r="N16" s="37" t="n"/>
       <c r="O16" s="37" t="n"/>
@@ -1994,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="Q16" s="37" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="R16" s="37" t="n"/>
       <c r="S16" s="37" t="n"/>
@@ -2004,68 +2025,52 @@
       <c r="W16" s="37" t="n"/>
       <c r="X16" s="37" t="n"/>
       <c r="Y16" s="37" t="n"/>
-      <c r="Z16" s="37" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA16" s="37" t="n">
-        <v>123</v>
-      </c>
+      <c r="Z16" s="37" t="n"/>
+      <c r="AA16" s="37" t="n"/>
       <c r="AB16" s="37" t="n"/>
       <c r="AC16" s="37" t="n"/>
       <c r="AD16" s="37" t="n">
         <v>1</v>
       </c>
       <c r="AE16" s="37" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AF16" s="37" t="n">
-        <v>1057</v>
+        <v>373</v>
       </c>
       <c r="AG16" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH16" s="37" t="n">
-        <v>1057</v>
+        <v>373</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="17">
       <c r="A17" s="37" t="inlineStr">
         <is>
-          <t>2020-06-25</t>
+          <t>2020-06-26</t>
         </is>
       </c>
       <c r="B17" s="37" t="n">
-        <v>1057</v>
+        <v>373</v>
       </c>
       <c r="C17" s="37" t="inlineStr"/>
       <c r="D17" s="37" t="n">
-        <v>1057</v>
+        <v>373</v>
       </c>
       <c r="E17" s="37" t="inlineStr"/>
-      <c r="F17" s="37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="F17" s="37" t="inlineStr"/>
       <c r="G17" s="37" t="n"/>
       <c r="H17" s="37" t="n"/>
       <c r="I17" s="37" t="n"/>
       <c r="J17" s="37" t="n"/>
       <c r="K17" s="37" t="n"/>
-      <c r="L17" s="37" t="inlineStr">
-        <is>
-          <t>682(682)</t>
-        </is>
-      </c>
+      <c r="L17" s="37" t="inlineStr"/>
       <c r="M17" s="37" t="n"/>
       <c r="N17" s="37" t="n"/>
       <c r="O17" s="37" t="n"/>
-      <c r="P17" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="37" t="n">
-        <v>26</v>
-      </c>
+      <c r="P17" s="37" t="n"/>
+      <c r="Q17" s="37" t="n"/>
       <c r="R17" s="37" t="n"/>
       <c r="S17" s="37" t="n"/>
       <c r="T17" s="37" t="n"/>
@@ -2074,16 +2079,12 @@
       <c r="W17" s="37" t="n"/>
       <c r="X17" s="37" t="n"/>
       <c r="Y17" s="37" t="n"/>
-      <c r="Z17" s="37" t="inlineStr"/>
-      <c r="AA17" s="37" t="inlineStr"/>
+      <c r="Z17" s="37" t="n"/>
+      <c r="AA17" s="37" t="n"/>
       <c r="AB17" s="37" t="n"/>
       <c r="AC17" s="37" t="n"/>
-      <c r="AD17" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="37" t="n">
-        <v>15</v>
-      </c>
+      <c r="AD17" s="37" t="n"/>
+      <c r="AE17" s="37" t="n"/>
       <c r="AF17" s="37" t="n">
         <v>373</v>
       </c>
@@ -2097,7 +2098,7 @@
     <row customHeight="1" ht="16.5" r="18">
       <c r="A18" s="37" t="inlineStr">
         <is>
-          <t>2020-06-26</t>
+          <t>2020-06-27</t>
         </is>
       </c>
       <c r="B18" s="37" t="n">
@@ -2118,8 +2119,8 @@
       <c r="M18" s="37" t="n"/>
       <c r="N18" s="37" t="n"/>
       <c r="O18" s="37" t="n"/>
-      <c r="P18" s="37" t="inlineStr"/>
-      <c r="Q18" s="37" t="inlineStr"/>
+      <c r="P18" s="37" t="n"/>
+      <c r="Q18" s="37" t="n"/>
       <c r="R18" s="37" t="n"/>
       <c r="S18" s="37" t="n"/>
       <c r="T18" s="37" t="n"/>
@@ -2128,12 +2129,12 @@
       <c r="W18" s="37" t="n"/>
       <c r="X18" s="37" t="n"/>
       <c r="Y18" s="37" t="n"/>
-      <c r="Z18" s="37" t="inlineStr"/>
-      <c r="AA18" s="37" t="inlineStr"/>
+      <c r="Z18" s="37" t="n"/>
+      <c r="AA18" s="37" t="n"/>
       <c r="AB18" s="37" t="n"/>
       <c r="AC18" s="37" t="n"/>
-      <c r="AD18" s="37" t="inlineStr"/>
-      <c r="AE18" s="37" t="inlineStr"/>
+      <c r="AD18" s="37" t="n"/>
+      <c r="AE18" s="37" t="n"/>
       <c r="AF18" s="37" t="n">
         <v>373</v>
       </c>
@@ -2147,7 +2148,7 @@
     <row customHeight="1" ht="16.5" r="19">
       <c r="A19" s="37" t="inlineStr">
         <is>
-          <t>2020-06-27</t>
+          <t>2020-06-28</t>
         </is>
       </c>
       <c r="B19" s="37" t="n">
@@ -2158,7 +2159,11 @@
         <v>373</v>
       </c>
       <c r="E19" s="37" t="inlineStr"/>
-      <c r="F19" s="37" t="inlineStr"/>
+      <c r="F19" s="37" t="inlineStr">
+        <is>
+          <t>636</t>
+        </is>
+      </c>
       <c r="G19" s="37" t="n"/>
       <c r="H19" s="37" t="n"/>
       <c r="I19" s="37" t="n"/>
@@ -2168,8 +2173,8 @@
       <c r="M19" s="37" t="n"/>
       <c r="N19" s="37" t="n"/>
       <c r="O19" s="37" t="n"/>
-      <c r="P19" s="37" t="inlineStr"/>
-      <c r="Q19" s="37" t="inlineStr"/>
+      <c r="P19" s="37" t="n"/>
+      <c r="Q19" s="37" t="n"/>
       <c r="R19" s="37" t="n"/>
       <c r="S19" s="37" t="n"/>
       <c r="T19" s="37" t="n"/>
@@ -2178,41 +2183,37 @@
       <c r="W19" s="37" t="n"/>
       <c r="X19" s="37" t="n"/>
       <c r="Y19" s="37" t="n"/>
-      <c r="Z19" s="37" t="inlineStr"/>
-      <c r="AA19" s="37" t="inlineStr"/>
+      <c r="Z19" s="37" t="n"/>
+      <c r="AA19" s="37" t="n"/>
       <c r="AB19" s="37" t="n"/>
       <c r="AC19" s="37" t="n"/>
-      <c r="AD19" s="37" t="inlineStr"/>
-      <c r="AE19" s="37" t="inlineStr"/>
+      <c r="AD19" s="37" t="n"/>
+      <c r="AE19" s="37" t="n"/>
       <c r="AF19" s="37" t="n">
-        <v>373</v>
+        <v>1009</v>
       </c>
       <c r="AG19" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH19" s="37" t="n">
-        <v>373</v>
+        <v>1009</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="20">
       <c r="A20" s="37" t="inlineStr">
         <is>
-          <t>2020-06-28</t>
+          <t>2020-06-29</t>
         </is>
       </c>
       <c r="B20" s="37" t="n">
-        <v>373</v>
+        <v>1009</v>
       </c>
       <c r="C20" s="37" t="inlineStr"/>
       <c r="D20" s="37" t="n">
-        <v>373</v>
+        <v>1009</v>
       </c>
       <c r="E20" s="37" t="inlineStr"/>
-      <c r="F20" s="37" t="inlineStr">
-        <is>
-          <t>636</t>
-        </is>
-      </c>
+      <c r="F20" s="37" t="inlineStr"/>
       <c r="G20" s="37" t="n"/>
       <c r="H20" s="37" t="n"/>
       <c r="I20" s="37" t="n"/>
@@ -2222,8 +2223,12 @@
       <c r="M20" s="37" t="n"/>
       <c r="N20" s="37" t="n"/>
       <c r="O20" s="37" t="n"/>
-      <c r="P20" s="37" t="inlineStr"/>
-      <c r="Q20" s="37" t="inlineStr"/>
+      <c r="P20" s="37" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="37" t="n">
+        <v>38</v>
+      </c>
       <c r="R20" s="37" t="n"/>
       <c r="S20" s="37" t="n"/>
       <c r="T20" s="37" t="n"/>
@@ -2232,34 +2237,38 @@
       <c r="W20" s="37" t="n"/>
       <c r="X20" s="37" t="n"/>
       <c r="Y20" s="37" t="n"/>
-      <c r="Z20" s="37" t="inlineStr"/>
-      <c r="AA20" s="37" t="inlineStr"/>
+      <c r="Z20" s="37" t="n"/>
+      <c r="AA20" s="37" t="n"/>
       <c r="AB20" s="37" t="n"/>
       <c r="AC20" s="37" t="n"/>
-      <c r="AD20" s="37" t="inlineStr"/>
-      <c r="AE20" s="37" t="inlineStr"/>
+      <c r="AD20" s="37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="37" t="n">
+        <v>28</v>
+      </c>
       <c r="AF20" s="37" t="n">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="AG20" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH20" s="37" t="n">
-        <v>1009</v>
+        <v>1003</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="21">
       <c r="A21" s="37" t="inlineStr">
         <is>
-          <t>2020-06-29</t>
+          <t>2020-06-30</t>
         </is>
       </c>
       <c r="B21" s="37" t="n">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="C21" s="37" t="inlineStr"/>
       <c r="D21" s="37" t="n">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="E21" s="37" t="inlineStr"/>
       <c r="F21" s="37" t="inlineStr"/>
@@ -2272,12 +2281,8 @@
       <c r="M21" s="37" t="n"/>
       <c r="N21" s="37" t="n"/>
       <c r="O21" s="37" t="n"/>
-      <c r="P21" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="37" t="n">
-        <v>38</v>
-      </c>
+      <c r="P21" s="37" t="n"/>
+      <c r="Q21" s="37" t="n"/>
       <c r="R21" s="37" t="n"/>
       <c r="S21" s="37" t="n"/>
       <c r="T21" s="37" t="n"/>
@@ -2286,16 +2291,12 @@
       <c r="W21" s="37" t="n"/>
       <c r="X21" s="37" t="n"/>
       <c r="Y21" s="37" t="n"/>
-      <c r="Z21" s="37" t="inlineStr"/>
-      <c r="AA21" s="37" t="inlineStr"/>
+      <c r="Z21" s="37" t="n"/>
+      <c r="AA21" s="37" t="n"/>
       <c r="AB21" s="37" t="n"/>
       <c r="AC21" s="37" t="n"/>
-      <c r="AD21" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE21" s="37" t="n">
-        <v>28</v>
-      </c>
+      <c r="AD21" s="37" t="n"/>
+      <c r="AE21" s="37" t="n"/>
       <c r="AF21" s="37" t="n">
         <v>1003</v>
       </c>
@@ -2309,7 +2310,7 @@
     <row customHeight="1" ht="16.5" r="22">
       <c r="A22" s="37" t="inlineStr">
         <is>
-          <t>2020-06-30</t>
+          <t>2020-07-01</t>
         </is>
       </c>
       <c r="B22" s="37" t="n">
@@ -2330,8 +2331,12 @@
       <c r="M22" s="37" t="n"/>
       <c r="N22" s="37" t="n"/>
       <c r="O22" s="37" t="n"/>
-      <c r="P22" s="37" t="inlineStr"/>
-      <c r="Q22" s="37" t="inlineStr"/>
+      <c r="P22" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="37" t="n">
+        <v>30</v>
+      </c>
       <c r="R22" s="37" t="n"/>
       <c r="S22" s="37" t="n"/>
       <c r="T22" s="37" t="n"/>
@@ -2340,51 +2345,61 @@
       <c r="W22" s="37" t="n"/>
       <c r="X22" s="37" t="n"/>
       <c r="Y22" s="37" t="n"/>
-      <c r="Z22" s="37" t="inlineStr"/>
-      <c r="AA22" s="37" t="inlineStr"/>
+      <c r="Z22" s="37" t="n"/>
+      <c r="AA22" s="37" t="n"/>
       <c r="AB22" s="37" t="n"/>
       <c r="AC22" s="37" t="n"/>
-      <c r="AD22" s="37" t="inlineStr"/>
-      <c r="AE22" s="37" t="inlineStr"/>
+      <c r="AD22" s="37" t="n"/>
+      <c r="AE22" s="37" t="n"/>
       <c r="AF22" s="37" t="n">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="AG22" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH22" s="37" t="n">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="23">
       <c r="A23" s="37" t="inlineStr">
         <is>
-          <t>2020-07-01</t>
+          <t>2020-07-02</t>
         </is>
       </c>
       <c r="B23" s="37" t="n">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C23" s="37" t="inlineStr"/>
       <c r="D23" s="37" t="n">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E23" s="37" t="inlineStr"/>
-      <c r="F23" s="37" t="inlineStr"/>
-      <c r="G23" s="37" t="n"/>
+      <c r="F23" s="37" t="inlineStr">
+        <is>
+          <t>(636)</t>
+        </is>
+      </c>
+      <c r="G23" s="37" t="n">
+        <v>4770</v>
+      </c>
       <c r="H23" s="37" t="n"/>
       <c r="I23" s="37" t="n"/>
       <c r="J23" s="37" t="n"/>
       <c r="K23" s="37" t="n"/>
-      <c r="L23" s="37" t="inlineStr"/>
+      <c r="L23" s="37" t="inlineStr">
+        <is>
+          <t>641(641)</t>
+        </is>
+      </c>
       <c r="M23" s="37" t="n"/>
       <c r="N23" s="37" t="n"/>
       <c r="O23" s="37" t="n"/>
       <c r="P23" s="37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="37" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R23" s="37" t="n"/>
       <c r="S23" s="37" t="n"/>
@@ -2394,62 +2409,52 @@
       <c r="W23" s="37" t="n"/>
       <c r="X23" s="37" t="n"/>
       <c r="Y23" s="37" t="n"/>
-      <c r="Z23" s="37" t="inlineStr"/>
-      <c r="AA23" s="37" t="inlineStr"/>
+      <c r="Z23" s="37" t="n"/>
+      <c r="AA23" s="37" t="n"/>
       <c r="AB23" s="37" t="n"/>
       <c r="AC23" s="37" t="n"/>
-      <c r="AD23" s="37" t="inlineStr"/>
-      <c r="AE23" s="37" t="inlineStr"/>
+      <c r="AD23" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="37" t="n">
+        <v>20</v>
+      </c>
       <c r="AF23" s="37" t="n">
-        <v>1001</v>
+        <v>358</v>
       </c>
       <c r="AG23" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH23" s="37" t="n">
-        <v>1001</v>
+        <v>358</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="24">
       <c r="A24" s="37" t="inlineStr">
         <is>
-          <t>2020-07-02</t>
+          <t>2020-07-03</t>
         </is>
       </c>
       <c r="B24" s="37" t="n">
-        <v>1001</v>
+        <v>358</v>
       </c>
       <c r="C24" s="37" t="inlineStr"/>
       <c r="D24" s="37" t="n">
-        <v>1001</v>
+        <v>358</v>
       </c>
       <c r="E24" s="37" t="inlineStr"/>
-      <c r="F24" s="37" t="inlineStr">
-        <is>
-          <t>(636)</t>
-        </is>
-      </c>
-      <c r="G24" s="37" t="n">
-        <v>4770</v>
-      </c>
+      <c r="F24" s="37" t="inlineStr"/>
+      <c r="G24" s="37" t="n"/>
       <c r="H24" s="37" t="n"/>
       <c r="I24" s="37" t="n"/>
       <c r="J24" s="37" t="n"/>
       <c r="K24" s="37" t="n"/>
-      <c r="L24" s="37" t="inlineStr">
-        <is>
-          <t>641(641)</t>
-        </is>
-      </c>
+      <c r="L24" s="37" t="inlineStr"/>
       <c r="M24" s="37" t="n"/>
       <c r="N24" s="37" t="n"/>
       <c r="O24" s="37" t="n"/>
-      <c r="P24" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="37" t="n">
-        <v>25</v>
-      </c>
+      <c r="P24" s="37" t="n"/>
+      <c r="Q24" s="37" t="n"/>
       <c r="R24" s="37" t="n"/>
       <c r="S24" s="37" t="n"/>
       <c r="T24" s="37" t="n"/>
@@ -2458,16 +2463,12 @@
       <c r="W24" s="37" t="n"/>
       <c r="X24" s="37" t="n"/>
       <c r="Y24" s="37" t="n"/>
-      <c r="Z24" s="37" t="inlineStr"/>
-      <c r="AA24" s="37" t="inlineStr"/>
+      <c r="Z24" s="37" t="n"/>
+      <c r="AA24" s="37" t="n"/>
       <c r="AB24" s="37" t="n"/>
       <c r="AC24" s="37" t="n"/>
-      <c r="AD24" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="37" t="n">
-        <v>20</v>
-      </c>
+      <c r="AD24" s="37" t="n"/>
+      <c r="AE24" s="37" t="n"/>
       <c r="AF24" s="37" t="n">
         <v>358</v>
       </c>
@@ -2481,7 +2482,7 @@
     <row customHeight="1" ht="16.5" r="25">
       <c r="A25" s="37" t="inlineStr">
         <is>
-          <t>2020-07-03</t>
+          <t>2020-07-04</t>
         </is>
       </c>
       <c r="B25" s="37" t="n">
@@ -2492,8 +2493,14 @@
         <v>358</v>
       </c>
       <c r="E25" s="37" t="inlineStr"/>
-      <c r="F25" s="37" t="inlineStr"/>
-      <c r="G25" s="37" t="n"/>
+      <c r="F25" s="37" t="inlineStr">
+        <is>
+          <t>655(655)</t>
+        </is>
+      </c>
+      <c r="G25" s="37" t="n">
+        <v>5197</v>
+      </c>
       <c r="H25" s="37" t="n"/>
       <c r="I25" s="37" t="n"/>
       <c r="J25" s="37" t="n"/>
@@ -2502,8 +2509,12 @@
       <c r="M25" s="37" t="n"/>
       <c r="N25" s="37" t="n"/>
       <c r="O25" s="37" t="n"/>
-      <c r="P25" s="37" t="inlineStr"/>
-      <c r="Q25" s="37" t="inlineStr"/>
+      <c r="P25" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="37" t="n">
+        <v>8</v>
+      </c>
       <c r="R25" s="37" t="n"/>
       <c r="S25" s="37" t="n"/>
       <c r="T25" s="37" t="n"/>
@@ -2512,44 +2523,42 @@
       <c r="W25" s="37" t="n"/>
       <c r="X25" s="37" t="n"/>
       <c r="Y25" s="37" t="n"/>
-      <c r="Z25" s="37" t="inlineStr"/>
-      <c r="AA25" s="37" t="inlineStr"/>
+      <c r="Z25" s="37" t="n"/>
+      <c r="AA25" s="37" t="n"/>
       <c r="AB25" s="37" t="n"/>
       <c r="AC25" s="37" t="n"/>
-      <c r="AD25" s="37" t="inlineStr"/>
-      <c r="AE25" s="37" t="inlineStr"/>
+      <c r="AD25" s="37" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE25" s="37" t="n">
+        <v>30</v>
+      </c>
       <c r="AF25" s="37" t="n">
-        <v>358</v>
+        <v>1008</v>
       </c>
       <c r="AG25" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH25" s="37" t="n">
-        <v>358</v>
+        <v>1008</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="26">
       <c r="A26" s="37" t="inlineStr">
         <is>
-          <t>2020-07-04</t>
+          <t>2020-07-05</t>
         </is>
       </c>
       <c r="B26" s="37" t="n">
-        <v>358</v>
+        <v>1008</v>
       </c>
       <c r="C26" s="37" t="inlineStr"/>
       <c r="D26" s="37" t="n">
-        <v>358</v>
+        <v>1008</v>
       </c>
       <c r="E26" s="37" t="inlineStr"/>
-      <c r="F26" s="37" t="inlineStr">
-        <is>
-          <t>655(655)</t>
-        </is>
-      </c>
-      <c r="G26" s="37" t="n">
-        <v>5197</v>
-      </c>
+      <c r="F26" s="37" t="inlineStr"/>
+      <c r="G26" s="37" t="n"/>
       <c r="H26" s="37" t="n"/>
       <c r="I26" s="37" t="n"/>
       <c r="J26" s="37" t="n"/>
@@ -2572,38 +2581,34 @@
       <c r="W26" s="37" t="n"/>
       <c r="X26" s="37" t="n"/>
       <c r="Y26" s="37" t="n"/>
-      <c r="Z26" s="37" t="inlineStr"/>
-      <c r="AA26" s="37" t="inlineStr"/>
+      <c r="Z26" s="37" t="n"/>
+      <c r="AA26" s="37" t="n"/>
       <c r="AB26" s="37" t="n"/>
       <c r="AC26" s="37" t="n"/>
-      <c r="AD26" s="37" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE26" s="37" t="n">
-        <v>30</v>
-      </c>
+      <c r="AD26" s="37" t="n"/>
+      <c r="AE26" s="37" t="n"/>
       <c r="AF26" s="37" t="n">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="AG26" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH26" s="37" t="n">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="27">
       <c r="A27" s="37" t="inlineStr">
         <is>
-          <t>2020-07-05</t>
+          <t>2020-07-06</t>
         </is>
       </c>
       <c r="B27" s="37" t="n">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C27" s="37" t="inlineStr"/>
       <c r="D27" s="37" t="n">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E27" s="37" t="inlineStr"/>
       <c r="F27" s="37" t="inlineStr"/>
@@ -2617,10 +2622,10 @@
       <c r="N27" s="37" t="n"/>
       <c r="O27" s="37" t="n"/>
       <c r="P27" s="37" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q27" s="37" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="R27" s="37" t="n"/>
       <c r="S27" s="37" t="n"/>
@@ -2630,34 +2635,38 @@
       <c r="W27" s="37" t="n"/>
       <c r="X27" s="37" t="n"/>
       <c r="Y27" s="37" t="n"/>
-      <c r="Z27" s="37" t="inlineStr"/>
-      <c r="AA27" s="37" t="inlineStr"/>
+      <c r="Z27" s="37" t="n"/>
+      <c r="AA27" s="37" t="n"/>
       <c r="AB27" s="37" t="n"/>
       <c r="AC27" s="37" t="n"/>
-      <c r="AD27" s="37" t="inlineStr"/>
-      <c r="AE27" s="37" t="inlineStr"/>
+      <c r="AD27" s="37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE27" s="37" t="n">
+        <v>28</v>
+      </c>
       <c r="AF27" s="37" t="n">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="AG27" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH27" s="37" t="n">
-        <v>1007</v>
+        <v>1000</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="28">
       <c r="A28" s="37" t="inlineStr">
         <is>
-          <t>2020-07-06</t>
+          <t>2020-07-07</t>
         </is>
       </c>
       <c r="B28" s="37" t="n">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="C28" s="37" t="inlineStr"/>
       <c r="D28" s="37" t="n">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="E28" s="37" t="inlineStr"/>
       <c r="F28" s="37" t="inlineStr"/>
@@ -2671,10 +2680,10 @@
       <c r="N28" s="37" t="n"/>
       <c r="O28" s="37" t="n"/>
       <c r="P28" s="37" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="37" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="R28" s="37" t="n"/>
       <c r="S28" s="37" t="n"/>
@@ -2684,38 +2693,34 @@
       <c r="W28" s="37" t="n"/>
       <c r="X28" s="37" t="n"/>
       <c r="Y28" s="37" t="n"/>
-      <c r="Z28" s="37" t="inlineStr"/>
-      <c r="AA28" s="37" t="inlineStr"/>
+      <c r="Z28" s="37" t="n"/>
+      <c r="AA28" s="37" t="n"/>
       <c r="AB28" s="37" t="n"/>
       <c r="AC28" s="37" t="n"/>
-      <c r="AD28" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE28" s="37" t="n">
-        <v>28</v>
-      </c>
+      <c r="AD28" s="37" t="n"/>
+      <c r="AE28" s="37" t="n"/>
       <c r="AF28" s="37" t="n">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="AG28" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH28" s="37" t="n">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="29">
       <c r="A29" s="37" t="inlineStr">
         <is>
-          <t>2020-07-07</t>
+          <t>2020-07-08</t>
         </is>
       </c>
       <c r="B29" s="37" t="n">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C29" s="37" t="inlineStr"/>
       <c r="D29" s="37" t="n">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E29" s="37" t="inlineStr"/>
       <c r="F29" s="37" t="inlineStr"/>
@@ -2732,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="Q29" s="37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R29" s="37" t="n"/>
       <c r="S29" s="37" t="n"/>
@@ -2742,34 +2747,38 @@
       <c r="W29" s="37" t="n"/>
       <c r="X29" s="37" t="n"/>
       <c r="Y29" s="37" t="n"/>
-      <c r="Z29" s="37" t="inlineStr"/>
-      <c r="AA29" s="37" t="inlineStr"/>
+      <c r="Z29" s="37" t="n"/>
+      <c r="AA29" s="37" t="n"/>
       <c r="AB29" s="37" t="n"/>
       <c r="AC29" s="37" t="n"/>
-      <c r="AD29" s="37" t="inlineStr"/>
-      <c r="AE29" s="37" t="inlineStr"/>
+      <c r="AD29" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="37" t="n">
+        <v>10</v>
+      </c>
       <c r="AF29" s="37" t="n">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="AG29" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH29" s="37" t="n">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="30">
       <c r="A30" s="37" t="inlineStr">
         <is>
-          <t>2020-07-08</t>
+          <t>2020-07-09</t>
         </is>
       </c>
       <c r="B30" s="37" t="n">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C30" s="37" t="inlineStr"/>
       <c r="D30" s="37" t="n">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E30" s="37" t="inlineStr"/>
       <c r="F30" s="37" t="inlineStr"/>
@@ -2778,15 +2787,19 @@
       <c r="I30" s="37" t="n"/>
       <c r="J30" s="37" t="n"/>
       <c r="K30" s="37" t="n"/>
-      <c r="L30" s="37" t="inlineStr"/>
+      <c r="L30" s="37" t="inlineStr">
+        <is>
+          <t>677(677)</t>
+        </is>
+      </c>
       <c r="M30" s="37" t="n"/>
       <c r="N30" s="37" t="n"/>
       <c r="O30" s="37" t="n"/>
       <c r="P30" s="37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q30" s="37" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R30" s="37" t="n"/>
       <c r="S30" s="37" t="n"/>
@@ -2796,38 +2809,38 @@
       <c r="W30" s="37" t="n"/>
       <c r="X30" s="37" t="n"/>
       <c r="Y30" s="37" t="n"/>
-      <c r="Z30" s="37" t="inlineStr"/>
-      <c r="AA30" s="37" t="inlineStr"/>
+      <c r="Z30" s="37" t="n"/>
+      <c r="AA30" s="37" t="n"/>
       <c r="AB30" s="37" t="n"/>
       <c r="AC30" s="37" t="n"/>
       <c r="AD30" s="37" t="n">
         <v>1</v>
       </c>
       <c r="AE30" s="37" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AF30" s="37" t="n">
-        <v>997</v>
+        <v>316</v>
       </c>
       <c r="AG30" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH30" s="37" t="n">
-        <v>997</v>
+        <v>316</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="31">
       <c r="A31" s="37" t="inlineStr">
         <is>
-          <t>2020-07-09</t>
+          <t>2020-07-10</t>
         </is>
       </c>
       <c r="B31" s="37" t="n">
-        <v>997</v>
+        <v>316</v>
       </c>
       <c r="C31" s="37" t="inlineStr"/>
       <c r="D31" s="37" t="n">
-        <v>997</v>
+        <v>316</v>
       </c>
       <c r="E31" s="37" t="inlineStr"/>
       <c r="F31" s="37" t="inlineStr"/>
@@ -2836,19 +2849,15 @@
       <c r="I31" s="37" t="n"/>
       <c r="J31" s="37" t="n"/>
       <c r="K31" s="37" t="n"/>
-      <c r="L31" s="37" t="inlineStr">
-        <is>
-          <t>677(677)</t>
-        </is>
-      </c>
+      <c r="L31" s="37" t="inlineStr"/>
       <c r="M31" s="37" t="n"/>
       <c r="N31" s="37" t="n"/>
       <c r="O31" s="37" t="n"/>
       <c r="P31" s="37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="37" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="R31" s="37" t="n"/>
       <c r="S31" s="37" t="n"/>
@@ -2858,42 +2867,48 @@
       <c r="W31" s="37" t="n"/>
       <c r="X31" s="37" t="n"/>
       <c r="Y31" s="37" t="n"/>
-      <c r="Z31" s="37" t="inlineStr"/>
-      <c r="AA31" s="37" t="inlineStr"/>
+      <c r="Z31" s="37" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA31" s="37" t="n">
+        <v>80</v>
+      </c>
       <c r="AB31" s="37" t="n"/>
       <c r="AC31" s="37" t="n"/>
-      <c r="AD31" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="37" t="n">
-        <v>5</v>
-      </c>
+      <c r="AD31" s="37" t="n"/>
+      <c r="AE31" s="37" t="n"/>
       <c r="AF31" s="37" t="n">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="AG31" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH31" s="37" t="n">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="32">
       <c r="A32" s="37" t="inlineStr">
         <is>
-          <t>2020-07-10</t>
+          <t>2020-07-11</t>
         </is>
       </c>
       <c r="B32" s="37" t="n">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C32" s="37" t="inlineStr"/>
       <c r="D32" s="37" t="n">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E32" s="37" t="inlineStr"/>
-      <c r="F32" s="37" t="inlineStr"/>
-      <c r="G32" s="37" t="n"/>
+      <c r="F32" s="37" t="inlineStr">
+        <is>
+          <t>694(694)</t>
+        </is>
+      </c>
+      <c r="G32" s="37" t="n">
+        <v>5321</v>
+      </c>
       <c r="H32" s="37" t="n"/>
       <c r="I32" s="37" t="n"/>
       <c r="J32" s="37" t="n"/>
@@ -2902,12 +2917,8 @@
       <c r="M32" s="37" t="n"/>
       <c r="N32" s="37" t="n"/>
       <c r="O32" s="37" t="n"/>
-      <c r="P32" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="37" t="n">
-        <v>9</v>
-      </c>
+      <c r="P32" s="37" t="n"/>
+      <c r="Q32" s="37" t="n"/>
       <c r="R32" s="37" t="n"/>
       <c r="S32" s="37" t="n"/>
       <c r="T32" s="37" t="n"/>
@@ -2916,48 +2927,38 @@
       <c r="W32" s="37" t="n"/>
       <c r="X32" s="37" t="n"/>
       <c r="Y32" s="37" t="n"/>
-      <c r="Z32" s="37" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA32" s="37" t="n">
-        <v>80</v>
-      </c>
+      <c r="Z32" s="37" t="n"/>
+      <c r="AA32" s="37" t="n"/>
       <c r="AB32" s="37" t="n"/>
       <c r="AC32" s="37" t="n"/>
-      <c r="AD32" s="37" t="inlineStr"/>
-      <c r="AE32" s="37" t="inlineStr"/>
+      <c r="AD32" s="37" t="n"/>
+      <c r="AE32" s="37" t="n"/>
       <c r="AF32" s="37" t="n">
-        <v>310</v>
+        <v>1004</v>
       </c>
       <c r="AG32" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH32" s="37" t="n">
-        <v>310</v>
+        <v>1004</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="33">
       <c r="A33" s="37" t="inlineStr">
         <is>
-          <t>2020-07-11</t>
+          <t>2020-07-12</t>
         </is>
       </c>
       <c r="B33" s="37" t="n">
-        <v>310</v>
+        <v>1004</v>
       </c>
       <c r="C33" s="37" t="inlineStr"/>
       <c r="D33" s="37" t="n">
-        <v>310</v>
+        <v>1004</v>
       </c>
       <c r="E33" s="37" t="inlineStr"/>
-      <c r="F33" s="37" t="inlineStr">
-        <is>
-          <t>694(694)</t>
-        </is>
-      </c>
-      <c r="G33" s="37" t="n">
-        <v>5321</v>
-      </c>
+      <c r="F33" s="37" t="inlineStr"/>
+      <c r="G33" s="37" t="n"/>
       <c r="H33" s="37" t="n"/>
       <c r="I33" s="37" t="n"/>
       <c r="J33" s="37" t="n"/>
@@ -2966,8 +2967,12 @@
       <c r="M33" s="37" t="n"/>
       <c r="N33" s="37" t="n"/>
       <c r="O33" s="37" t="n"/>
-      <c r="P33" s="37" t="inlineStr"/>
-      <c r="Q33" s="37" t="inlineStr"/>
+      <c r="P33" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="37" t="n">
+        <v>14</v>
+      </c>
       <c r="R33" s="37" t="n"/>
       <c r="S33" s="37" t="n"/>
       <c r="T33" s="37" t="n"/>
@@ -2976,34 +2981,34 @@
       <c r="W33" s="37" t="n"/>
       <c r="X33" s="37" t="n"/>
       <c r="Y33" s="37" t="n"/>
-      <c r="Z33" s="37" t="inlineStr"/>
-      <c r="AA33" s="37" t="inlineStr"/>
+      <c r="Z33" s="37" t="n"/>
+      <c r="AA33" s="37" t="n"/>
       <c r="AB33" s="37" t="n"/>
       <c r="AC33" s="37" t="n"/>
-      <c r="AD33" s="37" t="inlineStr"/>
-      <c r="AE33" s="37" t="inlineStr"/>
+      <c r="AD33" s="37" t="n"/>
+      <c r="AE33" s="37" t="n"/>
       <c r="AF33" s="37" t="n">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="AG33" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH33" s="37" t="n">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="34">
       <c r="A34" s="37" t="inlineStr">
         <is>
-          <t>2020-07-12</t>
+          <t>2020-07-13</t>
         </is>
       </c>
       <c r="B34" s="37" t="n">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C34" s="37" t="inlineStr"/>
       <c r="D34" s="37" t="n">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E34" s="37" t="inlineStr"/>
       <c r="F34" s="37" t="inlineStr"/>
@@ -3020,7 +3025,7 @@
         <v>2</v>
       </c>
       <c r="Q34" s="37" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="R34" s="37" t="n"/>
       <c r="S34" s="37" t="n"/>
@@ -3030,34 +3035,38 @@
       <c r="W34" s="37" t="n"/>
       <c r="X34" s="37" t="n"/>
       <c r="Y34" s="37" t="n"/>
-      <c r="Z34" s="37" t="inlineStr"/>
-      <c r="AA34" s="37" t="inlineStr"/>
+      <c r="Z34" s="37" t="n"/>
+      <c r="AA34" s="37" t="n"/>
       <c r="AB34" s="37" t="n"/>
       <c r="AC34" s="37" t="n"/>
-      <c r="AD34" s="37" t="inlineStr"/>
-      <c r="AE34" s="37" t="inlineStr"/>
+      <c r="AD34" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="37" t="n">
+        <v>7</v>
+      </c>
       <c r="AF34" s="37" t="n">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="AG34" s="37" t="n">
         <v>0</v>
       </c>
       <c r="AH34" s="37" t="n">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row customHeight="1" ht="16.5" r="35">
       <c r="A35" s="37" t="inlineStr">
         <is>
-          <t>2020-07-13</t>
+          <t>2020-07-14</t>
         </is>
       </c>
       <c r="B35" s="37" t="n">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C35" s="37" t="inlineStr"/>
       <c r="D35" s="37" t="n">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="E35" s="37" t="inlineStr"/>
       <c r="F35" s="37" t="inlineStr"/>
@@ -3070,12 +3079,8 @@
       <c r="M35" s="37" t="n"/>
       <c r="N35" s="37" t="n"/>
       <c r="O35" s="37" t="n"/>
-      <c r="P35" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q35" s="37" t="n">
-        <v>20</v>
-      </c>
+      <c r="P35" s="37" t="n"/>
+      <c r="Q35" s="37" t="n"/>
       <c r="R35" s="37" t="n"/>
       <c r="S35" s="37" t="n"/>
       <c r="T35" s="37" t="n"/>
@@ -3084,16 +3089,12 @@
       <c r="W35" s="37" t="n"/>
       <c r="X35" s="37" t="n"/>
       <c r="Y35" s="37" t="n"/>
-      <c r="Z35" s="37" t="inlineStr"/>
-      <c r="AA35" s="37" t="inlineStr"/>
+      <c r="Z35" s="37" t="n"/>
+      <c r="AA35" s="37" t="n"/>
       <c r="AB35" s="37" t="n"/>
       <c r="AC35" s="37" t="n"/>
-      <c r="AD35" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="37" t="n">
-        <v>7</v>
-      </c>
+      <c r="AD35" s="37" t="n"/>
+      <c r="AE35" s="37" t="n"/>
       <c r="AF35" s="37" t="n"/>
       <c r="AG35" s="37" t="n"/>
       <c r="AH35" s="37" t="n"/>
@@ -3110,11 +3111,11 @@
       <c r="E36" s="50" t="n"/>
       <c r="F36" s="50" t="inlineStr">
         <is>
-          <t>3255(3254)</t>
+          <t>2565(2564)</t>
         </is>
       </c>
       <c r="G36" s="50" t="n">
-        <v>25059.6</v>
+        <v>19746.6</v>
       </c>
       <c r="H36" s="50" t="n"/>
       <c r="I36" s="50" t="n"/>
@@ -3129,10 +3130,10 @@
       <c r="N36" s="50" t="n"/>
       <c r="O36" s="50" t="n"/>
       <c r="P36" s="50" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q36" s="50" t="n">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="R36" s="50" t="n"/>
       <c r="S36" s="50" t="n"/>
@@ -3151,10 +3152,10 @@
       <c r="AB36" s="50" t="n"/>
       <c r="AC36" s="50" t="n"/>
       <c r="AD36" s="50" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AE36" s="50" t="n">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="AF36" s="50" t="n"/>
       <c r="AG36" s="50" t="n"/>
@@ -3285,7 +3286,7 @@
       <c r="J40" s="37" t="n"/>
       <c r="K40" s="37" t="n"/>
       <c r="L40" s="37" t="n">
-        <v>2.089093701996928</v>
+        <v>2.53411306042885</v>
       </c>
       <c r="M40" s="37" t="n"/>
       <c r="N40" s="37" t="n"/>
@@ -3322,16 +3323,38 @@
       <c r="I41" s="37" t="n"/>
       <c r="J41" s="37" t="n"/>
       <c r="K41" s="37" t="n"/>
-      <c r="L41" s="37" t="n"/>
+      <c r="L41" s="37" t="inlineStr">
+        <is>
+          <t>Ср.вес 1 головы</t>
+        </is>
+      </c>
       <c r="M41" s="37" t="n"/>
       <c r="N41" s="37" t="n"/>
-      <c r="O41" s="37" t="n"/>
-      <c r="P41" s="37" t="n"/>
+      <c r="O41" s="37" t="inlineStr">
+        <is>
+          <t>падежа</t>
+        </is>
+      </c>
+      <c r="P41" s="37" t="n">
+        <v>10.6458333333333</v>
+      </c>
       <c r="Q41" s="37" t="n"/>
-      <c r="R41" s="37" t="n"/>
-      <c r="S41" s="37" t="n"/>
-      <c r="T41" s="37" t="n"/>
-      <c r="U41" s="37" t="n"/>
+      <c r="R41" s="37" t="inlineStr">
+        <is>
+          <t>прирезки</t>
+        </is>
+      </c>
+      <c r="S41" s="37" t="n">
+        <v>10.1818181818182</v>
+      </c>
+      <c r="T41" s="37" t="inlineStr">
+        <is>
+          <t>в.убой</t>
+        </is>
+      </c>
+      <c r="U41" s="37" t="n">
+        <v>13.88</v>
+      </c>
       <c r="V41" s="37" t="n"/>
       <c r="W41" s="37" t="n"/>
       <c r="X41" s="37" t="n"/>

</xml_diff>

<commit_message>
export to excel ws reports
</commit_message>
<xml_diff>
--- a/data/ws4_output.xlsx
+++ b/data/ws4_output.xlsx
@@ -1041,12 +1041,16 @@
       <c r="Q1" s="38" t="n"/>
       <c r="R1" s="18" t="inlineStr">
         <is>
-          <t>цех 4</t>
+          <t xml:space="preserve">в 8 цехе </t>
         </is>
       </c>
       <c r="S1" s="18" t="n"/>
       <c r="T1" s="23" t="n"/>
-      <c r="U1" s="23" t="n"/>
+      <c r="U1" s="23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="V1" s="19" t="n"/>
       <c r="W1" s="19" t="inlineStr">
         <is>
@@ -3121,10 +3125,8 @@
       <c r="I36" s="50" t="n"/>
       <c r="J36" s="50" t="n"/>
       <c r="K36" s="50" t="n"/>
-      <c r="L36" s="50" t="inlineStr">
-        <is>
-          <t>2632(2632)</t>
-        </is>
+      <c r="L36" s="50" t="n">
+        <v>2632</v>
       </c>
       <c r="M36" s="50" t="n"/>
       <c r="N36" s="50" t="n"/>
@@ -3151,12 +3153,8 @@
       </c>
       <c r="AB36" s="50" t="n"/>
       <c r="AC36" s="50" t="n"/>
-      <c r="AD36" s="50" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE36" s="50" t="n">
-        <v>189</v>
-      </c>
+      <c r="AD36" s="50" t="n"/>
+      <c r="AE36" s="50" t="n"/>
       <c r="AF36" s="50" t="n"/>
       <c r="AG36" s="50" t="n"/>
       <c r="AH36" s="50" t="n"/>

</xml_diff>